<commit_message>
Add get strut function.
</commit_message>
<xml_diff>
--- a/src/test/resources/project.xlsx
+++ b/src/test/resources/project.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SkyDrive\Work\ProjectDeveloping\EasyBI\excel2javabean-example\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\i\OneDrive\Enjoy_Projects\EZ\EZ-ExcelConverter\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="项目模块列表" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>模块</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -74,31 +74,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>分析</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分析功能一</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>合计价格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分析功能二</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>XXX项目</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>否</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>分析</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>分析功能一</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>合计价格</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>分析功能二</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>否</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>XXX项目</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -114,14 +110,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -130,7 +126,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -139,7 +135,7 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -449,7 +445,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -465,7 +461,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -510,9 +506,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -545,9 +541,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -730,10 +726,10 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.75" customWidth="1"/>
     <col min="2" max="2" width="17.875" customWidth="1"/>
@@ -744,9 +740,9 @@
     <col min="7" max="7" width="13.5" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -755,7 +751,7 @@
       <c r="F1" s="14"/>
       <c r="G1" s="14"/>
     </row>
-    <row r="2" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
@@ -774,7 +770,7 @@
       <c r="F2" s="19"/>
       <c r="G2" s="20"/>
     </row>
-    <row r="3" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="22"/>
       <c r="B3" s="23"/>
       <c r="C3" s="25"/>
@@ -789,7 +785,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>7</v>
       </c>
@@ -812,7 +808,7 @@
         <v>41400</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18"/>
       <c r="B5" s="7" t="s">
         <v>11</v>
@@ -827,16 +823,16 @@
         <v>0.59</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="C6" s="11">
         <v>2</v>
@@ -848,10 +844,10 @@
       <c r="F6" s="7"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="29"/>
       <c r="B7" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="11">
         <v>4</v>
@@ -863,15 +859,15 @@
         <v>0.01</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="G7" s="10">
         <v>41426</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="15">
         <f>SUM(D4:D7)</f>
@@ -896,6 +892,11 @@
     <mergeCell ref="A6:A7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F7">
+      <formula1>"是,否"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>